<commit_message>
Error handled with toast notification at login page
</commit_message>
<xml_diff>
--- a/public/Book2.xlsx
+++ b/public/Book2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nandu\Desktop\TH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nandu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C893191-4417-41BF-844C-CA5A62566DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354CF128-8923-4E8F-AB8E-149AAFCF58FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{98CC4610-9849-4AB2-9912-48A342A9CB30}"/>
   </bookViews>
@@ -408,11 +408,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB45746-7B61-4B64-8C4C-770B409133CC}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="49" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -421,12 +424,13 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>